<commit_message>
BUG Pseudorandomized Con Schedules
Making sure the Neg without UCS is never shown first
</commit_message>
<xml_diff>
--- a/2_Condition_Short.xlsx
+++ b/2_Condition_Short.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{932D0FF6-EF6E-4AF4-8F5F-60D18E581DBA}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C07F0086-6866-4585-9418-49A67BA23CA6}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,13 +138,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,10 +161,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,8 +487,8 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -500,7 +497,7 @@
     <col min="2" max="2" width="22.47265625" style="4" customWidth="1"/>
     <col min="3" max="3" width="19.83984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.47265625" style="4"/>
-    <col min="5" max="16384" width="8.83984375" style="4"/>
+    <col min="5" max="16384" width="8.83984375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
@@ -517,91 +514,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -615,21 +612,21 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -643,7 +640,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -657,49 +654,49 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -713,88 +710,88 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.6">
@@ -826,45 +823,45 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.4</v>
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.4</v>
+      <c r="A25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.4</v>
+      <c r="A26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.6">
@@ -882,87 +879,87 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.4</v>
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.4</v>
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.4</v>
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.4</v>
+      <c r="A31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.4</v>
+      <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.4</v>
+      <c r="A33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.6">
@@ -980,17 +977,17 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.4</v>
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.6">
@@ -1008,31 +1005,31 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.4</v>
+      <c r="A37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A38" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.4</v>
+      <c r="D38" s="4">
+        <v>0.9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.6">
@@ -1050,90 +1047,90 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0.4</v>
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A41" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A43" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D43" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A44" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A46" s="3" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A47" s="3" t="s">
         <v>8</v>
       </c>
@@ -1161,35 +1158,35 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A49" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D49" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
@@ -1203,35 +1200,35 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A53" s="3" t="s">
         <v>8</v>
       </c>
@@ -1245,105 +1242,105 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A54" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A55" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A56" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A58" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A59" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A61" s="3" t="s">
         <v>8</v>
       </c>
@@ -1359,16 +1356,16 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A62" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="4">
-        <v>0.9</v>
+      <c r="D62" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.6">
@@ -1386,17 +1383,17 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A64" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="4">
-        <v>0.9</v>
+      <c r="A64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -1405,9 +1402,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1595,26 +1595,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1638,9 +1627,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>